<commit_message>
tirei os threat sleep
</commit_message>
<xml_diff>
--- a/target/bancoDados.xlsx
+++ b/target/bancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.silva\eclipse-workspace\Appium_Hub_TDD\target\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D9E27C-1905-4BE1-AB08-553084BCB778}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F33D23B-9C52-4C25-A112-F979182EEEF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>Usuario</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>saulos71</t>
+  </si>
+  <si>
+    <t>pais</t>
+  </si>
+  <si>
+    <t>Brazil</t>
   </si>
 </sst>
 </file>
@@ -711,10 +717,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF751C6D-0313-48F7-A015-FFF3B2048B34}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -725,7 +731,7 @@
     <col min="5" max="5" width="26.26953125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,8 +765,11 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>56</v>
       </c>
@@ -794,8 +803,11 @@
       <c r="K2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -829,8 +841,11 @@
       <c r="K3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -838,7 +853,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -846,7 +861,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -854,7 +869,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -862,7 +877,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -870,7 +885,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -878,19 +893,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>55</v>
       </c>

</xml_diff>